<commit_message>
rowSums approach for NA problem
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_EPICP_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_EPICP_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715B0514-2251-46E3-AD6E-A36182738649}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAAE62-FD66-4EAF-8F35-5B4FB54EB13E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1096,10 +1096,10 @@
     <t>1(FFQ)</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>rowwise() %&gt;% TOBACCO_D = sum((zt3*1), (zr3*5),(pf3*5), na.rm = TRUE))</t>
+    <t>zt3;zr3pf3</t>
+  </si>
+  <si>
+    <t>rowSums(select(.,zt3*1,zr3*5,pf3*5), na.rm = TRUE)</t>
   </si>
 </sst>
 </file>
@@ -1871,10 +1871,10 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="G12" t="s">
-        <v>347</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
         <v>348</v>

</xml_diff>